<commit_message>
Promena na config za patekata
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalaj\Documents\UiPath\InvoiceProcessing1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{568554FF-DD0C-484F-9A95-403BCC99DF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6849BE61-C745-4AFC-8601-510D6928EC84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -258,9 +258,6 @@
     <t xml:space="preserve">Resuming after extraction validation for document: </t>
   </si>
   <si>
-    <t>Data\Exports\</t>
-  </si>
-  <si>
     <t>Data\ReceiptsTraining\</t>
   </si>
   <si>
@@ -511,6 +508,9 @@
   </si>
   <si>
     <t>C:\Users\kalaj\Documents\UiPath\InvoiceProcessing1\Data\ExampleDocuments\testInvoices2</t>
+  </si>
+  <si>
+    <t>C:\Users\kalaj\Documents\UiPath\InvoiceProcessing1\Data\Exports\</t>
   </si>
 </sst>
 </file>
@@ -897,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -973,13 +973,13 @@
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -987,7 +987,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>162</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -998,7 +998,7 @@
         <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" t="s">
         <v>69</v>
@@ -1009,7 +1009,7 @@
         <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C6" t="s">
         <v>70</v>
@@ -1018,13 +1018,13 @@
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" t="s">
         <v>139</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>140</v>
-      </c>
-      <c r="C8" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1033,10 +1033,10 @@
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1044,7 +1044,7 @@
         <v>39</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1052,40 +1052,40 @@
         <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1120,7 +1120,7 @@
         <v>59</v>
       </c>
       <c r="C20" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -1128,66 +1128,66 @@
         <v>5</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C21" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" t="s">
         <v>97</v>
       </c>
-      <c r="B23" t="s">
-        <v>98</v>
-      </c>
       <c r="C23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>150</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C25" t="s">
         <v>151</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="C25" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" t="s">
         <v>153</v>
       </c>
-      <c r="B26" t="s">
-        <v>154</v>
-      </c>
       <c r="C26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>154</v>
+      </c>
+      <c r="B27" t="s">
         <v>155</v>
       </c>
-      <c r="B27" t="s">
-        <v>156</v>
-      </c>
       <c r="C27" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2242,51 +2242,51 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B5" s="3">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B6" s="3">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" s="3">
         <v>30</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2297,7 +2297,7 @@
         <v>30</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2344,10 +2344,10 @@
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2360,10 +2360,10 @@
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2416,10 +2416,10 @@
     </row>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" t="s">
         <v>103</v>
-      </c>
-      <c r="B25" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2432,10 +2432,10 @@
     </row>
     <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" t="s">
         <v>81</v>
-      </c>
-      <c r="B27" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2448,10 +2448,10 @@
     </row>
     <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -2513,102 +2513,102 @@
     <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" t="s">
         <v>146</v>
-      </c>
-      <c r="B39" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>106</v>
+      </c>
+      <c r="B41" t="s">
         <v>107</v>
-      </c>
-      <c r="B41" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" t="s">
         <v>129</v>
-      </c>
-      <c r="B45" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>115</v>
+      </c>
+      <c r="B46" t="s">
         <v>116</v>
-      </c>
-      <c r="B46" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>117</v>
+      </c>
+      <c r="B47" t="s">
         <v>118</v>
-      </c>
-      <c r="B47" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>121</v>
+      </c>
+      <c r="B48" t="s">
         <v>122</v>
-      </c>
-      <c r="B48" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B49" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="52" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>111</v>
+      </c>
+      <c r="B52" t="s">
         <v>112</v>
-      </c>
-      <c r="B52" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" t="s">
         <v>114</v>
-      </c>
-      <c r="B53" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2617,7 +2617,7 @@
         <v>58</v>
       </c>
       <c r="B55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Commit with added mail to folder functionality
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kalaj\Documents\UiPath\InvoiceProcessing1\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A23266C4-6F5D-4BC5-928A-0B7E3869B056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0C0FD7-61C4-46A2-9CC0-29AF6FADA4FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="174">
   <si>
     <t>Name</t>
   </si>
@@ -538,6 +538,12 @@
   </si>
   <si>
     <t>C:\Users\kalaj\Documents\UiPath\InvoiceProcessing1\Data\Exports</t>
+  </si>
+  <si>
+    <t>MailList</t>
+  </si>
+  <si>
+    <t>kalajdziskabjanka@gmail.com,krpacovskamarija@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -596,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -607,6 +613,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -924,8 +931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1255,29 +1262,36 @@
       <c r="A32" t="s">
         <v>168</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="8" t="s">
         <v>164</v>
       </c>
       <c r="C32" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>172</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>